<commit_message>
added alot of additional metrics and mad changes to the text
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -948,7 +948,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Leg </t>
+          <t>Legs</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -1248,7 +1248,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Leg</t>
+          <t>Legs</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -2218,7 +2218,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Legs + Abdo </t>
+          <t xml:space="preserve">Legs + Core </t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -2874,7 +2874,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Running mix</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -4166,7 +4166,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Chest + abdo</t>
+          <t>Chest + Core</t>
         </is>
       </c>
       <c r="B126" t="inlineStr"/>
@@ -5060,7 +5060,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Run</t>
+          <t>Running</t>
         </is>
       </c>
       <c r="B157" t="inlineStr"/>

</xml_diff>